<commit_message>
att dicionario de dados
</commit_message>
<xml_diff>
--- a/documentacao/Banco de dados/dicionario de dados.xlsx
+++ b/documentacao/Banco de dados/dicionario de dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel alvares\Desktop\band tec\disciplinas 1S\Z_projeto P.I 3ªSPRINT\Cyberlife\documentacao\Banco de dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Documents\Bandtec\Pesquisa e Inovação\sprint\Cyberlife\documentacao\Banco de dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800F752A-C5BA-4412-8028-BDBB0D3B4850}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9F2429-D3A5-44C5-B2F8-D738BD3548BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B60625FA-F1DE-460A-A32A-4856CDA89F55}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{B60625FA-F1DE-460A-A32A-4856CDA89F55}"/>
   </bookViews>
   <sheets>
     <sheet name="DD entidade" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="163">
   <si>
     <t>atributo</t>
   </si>
@@ -413,9 +413,6 @@
   </si>
   <si>
     <t>data e hora da temperatura capturadas dentro da caixa</t>
-  </si>
-  <si>
-    <t>Volume esperado:</t>
   </si>
   <si>
     <t>Tempo de retenção:</t>
@@ -759,6 +756,42 @@
       </rPr>
       <t>dbo.usuario</t>
     </r>
+  </si>
+  <si>
+    <t>Tempo de retenção: permanente</t>
+  </si>
+  <si>
+    <t>Rotina de limpeza: Não se aplica</t>
+  </si>
+  <si>
+    <t>Volume esperado: 20 por mês</t>
+  </si>
+  <si>
+    <t>Volume esperado: 200 por mês</t>
+  </si>
+  <si>
+    <t>Tempo de retenção: 1 mês</t>
+  </si>
+  <si>
+    <t>Volume esperado: 2000 por mês</t>
+  </si>
+  <si>
+    <t>Volume esperado: 20 por ano</t>
+  </si>
+  <si>
+    <t>Volume esperado: 400 por mês</t>
+  </si>
+  <si>
+    <t>Rotina de limpeza: Uma vez a cada 5 anos</t>
+  </si>
+  <si>
+    <t>Rotina de limpeza: Uma vez a cada 1 ano</t>
+  </si>
+  <si>
+    <t>Rotina de limpeza:  Uma vez a cada 5 anos</t>
+  </si>
+  <si>
+    <t>Volume esperado: carga inicial de 60 ocorrências e volume mensal de 2 ocorrências</t>
   </si>
 </sst>
 </file>
@@ -1294,7 +1327,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7944ADE-D100-4E13-8EFA-A90EBA8EEC56}">
   <dimension ref="A1:A62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1311,32 +1346,32 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1350,32 +1385,32 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>128</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1389,32 +1424,32 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1422,7 +1457,7 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
@@ -1430,32 +1465,32 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1471,32 +1506,32 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1512,32 +1547,32 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1545,7 +1580,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -1553,32 +1588,32 @@
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1590,7 +1625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C066EE5-60CF-46E1-A675-28C9FF634E04}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
@@ -2060,7 +2095,7 @@
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2446,7 +2481,7 @@
     </row>
     <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>

</xml_diff>

<commit_message>
dicionario de dados completo
</commit_message>
<xml_diff>
--- a/documentacao/Banco de dados/dicionario de dados.xlsx
+++ b/documentacao/Banco de dados/dicionario de dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Documents\Bandtec\Pesquisa e Inovação\sprint\Cyberlife\documentacao\Banco de dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel alvares\Desktop\band tec\disciplinas 1S\Z_projeto P.I 3ªSPRINT\Cyberlife\documentacao\Banco de dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9F2429-D3A5-44C5-B2F8-D738BD3548BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB3534D-8EC2-416F-B03C-E24DF1B00208}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{B60625FA-F1DE-460A-A32A-4856CDA89F55}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B60625FA-F1DE-460A-A32A-4856CDA89F55}"/>
   </bookViews>
   <sheets>
     <sheet name="DD entidade" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="161">
   <si>
     <t>atributo</t>
   </si>
@@ -415,12 +415,6 @@
     <t>data e hora da temperatura capturadas dentro da caixa</t>
   </si>
   <si>
-    <t>Tempo de retenção:</t>
-  </si>
-  <si>
-    <t>Rotina de limpeza:</t>
-  </si>
-  <si>
     <t>entidade orgao</t>
   </si>
   <si>
@@ -758,40 +752,184 @@
     </r>
   </si>
   <si>
-    <t>Tempo de retenção: permanente</t>
-  </si>
-  <si>
-    <t>Rotina de limpeza: Não se aplica</t>
-  </si>
-  <si>
-    <t>Volume esperado: 20 por mês</t>
-  </si>
-  <si>
-    <t>Volume esperado: 200 por mês</t>
-  </si>
-  <si>
-    <t>Tempo de retenção: 1 mês</t>
-  </si>
-  <si>
-    <t>Volume esperado: 2000 por mês</t>
-  </si>
-  <si>
-    <t>Volume esperado: 20 por ano</t>
-  </si>
-  <si>
-    <t>Volume esperado: 400 por mês</t>
-  </si>
-  <si>
-    <t>Rotina de limpeza: Uma vez a cada 5 anos</t>
-  </si>
-  <si>
-    <t>Rotina de limpeza: Uma vez a cada 1 ano</t>
-  </si>
-  <si>
-    <t>Rotina de limpeza:  Uma vez a cada 5 anos</t>
-  </si>
-  <si>
-    <t>Volume esperado: carga inicial de 60 ocorrências e volume mensal de 2 ocorrências</t>
+    <r>
+      <t xml:space="preserve">Volume esperado: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>carga inicial de 60 ocorrências e volume mensal de 2 ocorrências</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rotina de limpeza: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Uma vez a cada 5 anos</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Volume esperado: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2000 por mês</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tempo de retenção: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 mês</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Volume esperado: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>400 por mês</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Volume esperado: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>20 por ano</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tempo de retenção: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>permanente</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rotina de limpeza: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Uma vez a cada 1 ano</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Volume esperado: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>200 por mês</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rotina de limpeza:  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Uma vez a cada 5 anos</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Volume esperado: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>20 por mês</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Rotina de limpeza: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Não se aplica</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1327,8 +1465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7944ADE-D100-4E13-8EFA-A90EBA8EEC56}">
   <dimension ref="A1:A62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,32 +1484,32 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1385,32 +1523,32 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1424,32 +1562,32 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1457,7 +1595,7 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
@@ -1465,32 +1603,32 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1506,32 +1644,32 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1547,32 +1685,32 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1580,7 +1718,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -1588,36 +1726,37 @@
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1625,8 +1764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C066EE5-60CF-46E1-A675-28C9FF634E04}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2095,7 +2234,7 @@
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2481,7 +2620,7 @@
     </row>
     <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>

</xml_diff>